<commit_message>
Adicionadas as estimativas COCOMO
</commit_message>
<xml_diff>
--- a/estimacao.xlsx
+++ b/estimacao.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudos\Fcul\Terceiro Ano\PGP\Proj2_Etapa1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudos\Fcul\Terceiro Ano\PGP\Proj2_Etapa1\PGP_Etapa_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2467B813-8C7F-47DD-9282-7E2C49999B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001DFE14-C225-44B1-9B93-7017A7B068C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB784219-E9DA-44A7-A6F6-7AA67144AE3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AB784219-E9DA-44A7-A6F6-7AA67144AE3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Linhas" sheetId="1" r:id="rId1"/>
+    <sheet name="COCOMO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>RF-ADMIN-1</t>
   </si>
@@ -97,6 +98,84 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Product Attributes</t>
+  </si>
+  <si>
+    <t>Required Reliability</t>
+  </si>
+  <si>
+    <t>1.00 (N )</t>
+  </si>
+  <si>
+    <t>Database Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	0.94 (L )</t>
+  </si>
+  <si>
+    <t>Product Complexity</t>
+  </si>
+  <si>
+    <t>1.15 (H )</t>
+  </si>
+  <si>
+    <t>Computer Attributes</t>
+  </si>
+  <si>
+    <t>Execution Time Constraint</t>
+  </si>
+  <si>
+    <t>Main Storage Constraint</t>
+  </si>
+  <si>
+    <t>Platform Volatility</t>
+  </si>
+  <si>
+    <t>Computer Turnaround Time</t>
+  </si>
+  <si>
+    <t>Personnel Attributes</t>
+  </si>
+  <si>
+    <t>Analyst Capability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	1.19 (L )</t>
+  </si>
+  <si>
+    <t>Applications Experience</t>
+  </si>
+  <si>
+    <t>1.13 (L )</t>
+  </si>
+  <si>
+    <t>Programmer Capability</t>
+  </si>
+  <si>
+    <t>Programming Language and Tool Experience</t>
+  </si>
+  <si>
+    <t>1.07 (L )</t>
+  </si>
+  <si>
+    <t>Platform Experience</t>
+  </si>
+  <si>
+    <t>Project Attributes</t>
+  </si>
+  <si>
+    <t>Modern Programming Practices</t>
+  </si>
+  <si>
+    <t>1.10 (L )</t>
+  </si>
+  <si>
+    <t>Use of Software Tools</t>
+  </si>
+  <si>
+    <t>Required Development Schedule</t>
   </si>
 </sst>
 </file>
@@ -133,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +243,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -309,6 +394,81 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -318,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +521,29 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -679,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535BB571-658C-496A-A045-01E7690595D0}">
   <dimension ref="E4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:I22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,4 +1236,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0056B5F2-2CED-43A8-995E-D1CA8B2EBBFE}">
+  <dimension ref="E4:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E20:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>